<commit_message>
correct the connector family type file
</commit_message>
<xml_diff>
--- a/Arent3d.Architecture.Routing.Electrical.App/resources/csv/ConnectorFamilyType.xlsx
+++ b/Arent3d.Architecture.Routing.Electrical.App/resources/csv/ConnectorFamilyType.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Family\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects R\architecture_routing\Arent3d.Architecture.Routing.Electrical.App\resources\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="131">
   <si>
     <t>〇</t>
   </si>
@@ -744,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,6 +981,9 @@
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="C29" s="2" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="30" spans="1:3" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">

</xml_diff>